<commit_message>
Update logging ass criteria
</commit_message>
<xml_diff>
--- a/Proj1_AbnormalLineDetect/Book1.xlsx
+++ b/Proj1_AbnormalLineDetect/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18255" windowHeight="7095" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18255" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,24 +663,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="90705920"/>
-        <c:axId val="90707456"/>
+        <c:axId val="80911744"/>
+        <c:axId val="60023936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90705920"/>
+        <c:axId val="80911744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90707456"/>
+        <c:crossAx val="60023936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90707456"/>
+        <c:axId val="60023936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +688,1182 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90705920"/>
+        <c:crossAx val="80911744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$1:$P$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="87"/>
+                <c:pt idx="0">
+                  <c:v>8.1078030000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3812900000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6818640000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6251699999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3351319999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8792249999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6950279999999989</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6885049999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5321720000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1180839999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3038779999999992</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1452489999999989</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2525050000000011</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6449449999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8163939999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.7151380000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8046179999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.6376790000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0203609999999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2520490000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0997879999999993</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7420220000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.88393899999999981</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.4196249999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.84295800000000032</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.6505339999999995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0794509999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.0384989999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.89941599999999955</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0785480000000005</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.327407</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5871239999999993</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.6349309999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.4405519999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0736110000000005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.5742709999999995</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0871650000000006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.203558000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.3961199999999989</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.4474</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2018910000000007</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10.110747</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12.001766999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.128539</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12.332184999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.4067070000000008</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>17.970295</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.3754539999999995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.3981840000000005</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.5768870000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6.4524360000000005</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.247001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.6668649999999996</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.2839020000000003</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.7202380000000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.5511119999999998</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.3563600000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.803833</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.1883470000000012</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.7571229999999991</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.2865449999999994</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.8400160000000003</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.114541</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.4252419999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.1903389999999989</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.6737409999999997</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.6915560000000003</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.211214</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.4138449999999994</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.653327</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.0715500000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.3234159999999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.7936169999999994</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.4491759999999996</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.0090270000000006</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.7080209999999996</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.406695</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.5261389999999997</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.0230570000000005</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.3389870000000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.7553409999999996</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.2950769999999991</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.5610520000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.1580249999999994</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.25106300000000026</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>14.178978000000001</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$1:$Q$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="87"/>
+                <c:pt idx="0">
+                  <c:v>9.9242650000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3995110000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8607650000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.7278979999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2788149999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3283579999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5633079999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.5846029999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.3822869999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.6799099999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.5170519999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.2132919999999991</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.4431980000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.2648989999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.7666439999999994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.5232340000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.9333349999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.9588080000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.5105939999999993</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.8179920000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.6187799999999992</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.9102680000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.6368109999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.6283570000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.5796510000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.8193429999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.5879829999999995</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.2445310000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.6149609999999992</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.7359470000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.5834299999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.1820579999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.5645340000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.8318469999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.4084000000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.1141199999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.1555440000000008</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.1524680000000007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.4925859999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.8561040000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.0757030000000007</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11.092169</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.1578839999999992</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.7071850000000008</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10.346729</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14.958447</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>22.456527000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.1084429999999994</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10.615009000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.0125890000000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10.045524</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.3766429999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>9.3784639999999992</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8.4637370000000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10.064285</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8.262435</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.5595730000000003</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7.9174009999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.2459330000000008</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8.1490659999999995</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.5811159999999997</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.968744</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.1021590000000003</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.9130989999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.1717809999999993</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>8.0025230000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>11.745245000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.7964389999999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>10.615632</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8.5555070000000004</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.8405690000000003</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.9315220000000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.7693969999999997</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.0259079999999994</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.9805030000000006</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8.2480639999999994</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.736205</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.1198189999999997</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8.5431290000000004</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.2307050000000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.3464559999999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.2858029999999996</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.557696</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.2561979999999995</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7.0919410000000003</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>11.097859</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$1:$R$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="87"/>
+                <c:pt idx="0">
+                  <c:v>1.816462</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0182209999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1789009999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1027279999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.943683</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4491329999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8682800000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.8960980000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8501149999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5618259999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.2131740000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0680430000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.1906929999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6199539999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.9502499999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.8080959999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.128717</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.321129</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.4902329999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.5659429999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.5189919999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.1682459999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.752872</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.2087320000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.7366929999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.1688090000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.5085319999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.2060320000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.7155449999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.6573989999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.2560229999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.5949340000000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.9296030000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.3912950000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.3347889999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.5398490000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.0683790000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.9489099999999997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.0964660000000004</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.4087040000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.873812</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.98142200000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-2.8438829999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.57864599999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.9854560000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.5517399999999997</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.4862320000000002</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.7329889999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.216825</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.435702</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.5930879999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.1296419999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.7115989999999996</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.1798349999999997</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.3440469999999998</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.7113230000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.2032129999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6.1135679999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.0575859999999997</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.3919430000000004</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.2945710000000004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1287279999999997</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.9876180000000003</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.487857</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.9814420000000004</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.3287820000000004</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.0536890000000003</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.5852249999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.2017870000000004</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.9021800000000004</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.7690190000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.6081060000000003</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.9757800000000003</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.5767319999999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6.971476</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.5400429999999998</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.32951</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.59368</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.5200719999999999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.891718</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.5911150000000003</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.9907260000000004</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.9966439999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>7.0981730000000001</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.840878</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-3.0811190000000002</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="92016640"/>
+        <c:axId val="92019712"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92016640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92019712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="92019712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92016640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$1:$C$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="78"/>
+                <c:pt idx="0">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>416</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="60680064"/>
+        <c:axId val="60681600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="60680064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60681600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="60681600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60680064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -707,347 +1882,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$1:$B$87</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="87"/>
-                <c:pt idx="0">
-                  <c:v>2.1290179999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.3252109999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4134869999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.800117</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.3491390000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5208159999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5651570000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.3264339999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.877297</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0976219999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.3076850000000002</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.3358410000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.5869490000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.070238</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.658331</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.84485200000000005</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.59718099999999996</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.400074</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.68623100000000004</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.8909560000000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.7643260000000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.5895730000000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.091885</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.97045099999999995</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.3791380000000002</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.770019</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.8337340000000002</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.5093100000000002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.4549280000000002</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.84536500000000003</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.55230400000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.70461</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.55921600000000005</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.75985899999999995</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.54922199999999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2.6682730000000001</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.58232200000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.829036</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.2468710000000001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.54266800000000004</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.1947269999999999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2.7712089999999998</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4.972861</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.7292130000000001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.49031</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.0401470000000002</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.0639449999999999</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5.5933979999999996</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.132069</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>3.4623620000000002</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.93247500000000005</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3.4130150000000001</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.52946099999999996</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.5814299999999999</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1.9437310000000001</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4.6400240000000004</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.61636299999999999</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6.8069090000000001</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.53132199999999996</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>4.0646009999999997</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.59190200000000004</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>3.8786369999999999</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2.7804760000000002</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>4.0593070000000004</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>3.2964560000000001</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>3.6169319999999998</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.58874899999999997</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.83221699999999998</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.85168699999999997</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1.056011</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.76630900000000002</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>4.4160760000000003</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.68393499999999996</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>3.7510599999999998</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.707484</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>6.1921340000000002</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.708399</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>3.4193609999999999</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.70021699999999998</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>3.4671180000000001</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.91028200000000004</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>3.6250800000000001</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.74895199999999995</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>5.0020689999999997</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>2.7678660000000002</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>5.2641080000000002</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>4.1621379999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="48062848"/>
-        <c:axId val="48064384"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="48062848"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48064384"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="48064384"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48062848"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1068,20 +1916,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvPr id="6" name="图表 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1091,6 +1939,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1386,8 +2269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="D47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6536,8 +7419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -11443,6 +12326,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>